<commit_message>
skip data test in one testcase
</commit_message>
<xml_diff>
--- a/scripts_demo/myscript/gmail_login_003.xlsx
+++ b/scripts_demo/myscript/gmail_login_003.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="11745" windowHeight="6345" tabRatio="849" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11745" windowHeight="6345" tabRatio="849" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="List Case" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Description</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>The email or password you entered is incorrect.</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -575,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -736,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -777,7 +780,7 @@
         <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="E2" s="2"/>
     </row>

</xml_diff>